<commit_message>
Finalized and Proofread WMD Story
</commit_message>
<xml_diff>
--- a/Stories/WMDs.xlsx
+++ b/Stories/WMDs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\DECO3801-Synergistiscs\Stories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ianch\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC13D625-571E-4DDB-B29B-507B97092932}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610F1281-E5B0-457B-B692-F4D64A078FED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{19A45076-EEA2-4D9B-A3FE-00F263EB5362}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{19A45076-EEA2-4D9B-A3FE-00F263EB5362}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>New weapons to cause mass destruction</t>
   </si>
   <si>
-    <t>The discover of a hidden weapons facility in a neighbouring kindom brings shocking news to the world. No-one knows where or what is in the facility but after attempting to reach out to the kingdom's military commander for comment, his silence says everything.</t>
-  </si>
-  <si>
     <t>ADVISOR OPINION</t>
   </si>
   <si>
@@ -107,18 +104,9 @@
     <t>They are our allies and we have been at peace with them for over a century.</t>
   </si>
   <si>
-    <t>From our reports there are no new weapons being made anywhere.</t>
-  </si>
-  <si>
-    <t>We should start saving away food just in case.</t>
-  </si>
-  <si>
     <t>Maybe we should evacuate?</t>
   </si>
   <si>
-    <t>I was wondering if the alliance was a scheme to conceal their actual financial situation</t>
-  </si>
-  <si>
     <t>Maybe that is why the metal ingot and charcoal are so expensive now.</t>
   </si>
   <si>
@@ -129,9 +117,6 @@
   </si>
   <si>
     <t>I do not think our allies will go against our peace treaty agreement.</t>
-  </si>
-  <si>
-    <t>Maybe our enemy is tring to cast a bone between us to destroy our friendship!</t>
   </si>
   <si>
     <t>OUTCOME</t>
@@ -150,39 +135,18 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Yes, they are definately spying on us.</t>
-  </si>
-  <si>
     <t>Spies always get caught</t>
   </si>
   <si>
-    <t>A few more spies never hurt</t>
-  </si>
-  <si>
-    <t>Maybe have them steal us something good too</t>
-  </si>
-  <si>
-    <t>If they get caught, peace will be lost</t>
-  </si>
-  <si>
     <t>I could have the peddlers working out for information as well!</t>
   </si>
   <si>
-    <t>Should not we prioritize why we must spend so much for training our spies?</t>
-  </si>
-  <si>
-    <t>I do not want to risk my men just because the military commander is stating so.</t>
-  </si>
-  <si>
     <t>Maybe it is better to buy off their men for more information.</t>
   </si>
   <si>
     <t>No, this must be a trap to frame us for doubting them!</t>
   </si>
   <si>
-    <t>The spies are better our best men to avoid being captured!</t>
-  </si>
-  <si>
     <t>ACTION 2</t>
   </si>
   <si>
@@ -192,9 +156,6 @@
     <t>This is a very smart move.</t>
   </si>
   <si>
-    <t>I would expect to get anywhere</t>
-  </si>
-  <si>
     <t>We must be prepared with questions.</t>
   </si>
   <si>
@@ -210,18 +171,9 @@
     <t>Maybe hosting a banquet to show our sincerity.</t>
   </si>
   <si>
-    <t>We may have unccessary expenses just to cater the guests.</t>
-  </si>
-  <si>
-    <t>There may be a chance they will ambush us here!</t>
-  </si>
-  <si>
     <t>If the commanders die in our Kingdom, we will be in trouble!</t>
   </si>
   <si>
-    <t>We should welcome them wiith open arms and treat them like honorable guests.</t>
-  </si>
-  <si>
     <t>We could revise our agreement as well!</t>
   </si>
   <si>
@@ -237,24 +189,15 @@
     <t>We should find out what the weapon is first, before sending our men in blind.</t>
   </si>
   <si>
-    <t>Throughout history violence is only matched with violence</t>
-  </si>
-  <si>
     <t>In history, violence always resolves issues. One way or another.</t>
   </si>
   <si>
     <t>Just don’t send in the farmers.</t>
   </si>
   <si>
-    <t xml:space="preserve"> I was hoping never to live through a war</t>
-  </si>
-  <si>
     <t>I am not saying we are already high in military expenditure.</t>
   </si>
   <si>
-    <t>Why do we always how to resort to such a move?</t>
-  </si>
-  <si>
     <t>Insufficient intelligence preparation will only sacrifice our men.</t>
   </si>
   <si>
@@ -273,22 +216,12 @@
     <t>Release news of our own secret weapons program.</t>
   </si>
   <si>
-    <t xml:space="preserve">This may make the other kingom nervous
-</t>
-  </si>
-  <si>
     <t>Make them scared!</t>
   </si>
   <si>
     <t>Rumuors and rumours, when will it end.</t>
   </si>
   <si>
-    <t>A little lie never hurt anyone</t>
-  </si>
-  <si>
-    <t>Be sure to say our weapons are superior</t>
-  </si>
-  <si>
     <t xml:space="preserve"> I hope this isn’t true.</t>
   </si>
   <si>
@@ -307,17 +240,83 @@
     <t>Do you want to attract more attentions from our enemies?</t>
   </si>
   <si>
-    <t>It is not a secret if the other neighbouring Kingdoms know it.</t>
-  </si>
-  <si>
     <t>DUNGEON</t>
+  </si>
+  <si>
+    <t>The discover of a hidden weapons facility in a neighbouring kindom brings shocking news to the world. No-one knows where or what is in the facility but after attempting to reach out to the kingdom's military commander for comments, his silence says everything.</t>
+  </si>
+  <si>
+    <t>From our reports, there are no new weapons being made anywhere.</t>
+  </si>
+  <si>
+    <t>We should start saving and stockpile the food just in case.</t>
+  </si>
+  <si>
+    <t>I was wondering if the alliance was a scheme to conceal their real intention.</t>
+  </si>
+  <si>
+    <t>Maybe our enemy is trying to cast a bone between us to destroy our alliance!</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yes, they are definitely spying on us.</t>
+  </si>
+  <si>
+    <t>Sending a few more spies never hurts.</t>
+  </si>
+  <si>
+    <t>Maybe have them steal us something good too!</t>
+  </si>
+  <si>
+    <t>If they get caught, peace will be lost.</t>
+  </si>
+  <si>
+    <t>Shouldn't we be focusing why we must spend so much to train our spies?</t>
+  </si>
+  <si>
+    <t>I do not want to risk my men just because the military commander is stating so!</t>
+  </si>
+  <si>
+    <t>The spies are our best men to avoid being captured.</t>
+  </si>
+  <si>
+    <t>I would not expect this to get anywhere.</t>
+  </si>
+  <si>
+    <t>We may overspend just to cater the guests.</t>
+  </si>
+  <si>
+    <t>There might be a chance they will ambush us here!</t>
+  </si>
+  <si>
+    <t>We should welcome them with open arms and treat them like honorable guests.</t>
+  </si>
+  <si>
+    <t>Throughout history, violence is only matched with violence.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I was hoping never to live through a war.</t>
+  </si>
+  <si>
+    <t>Why do we always have to resort to such a move?</t>
+  </si>
+  <si>
+    <t>This may make the other kingom nervous.</t>
+  </si>
+  <si>
+    <t>A little lie will never hurt.</t>
+  </si>
+  <si>
+    <t>Be sure to say our weapons are more superior.</t>
+  </si>
+  <si>
+    <t>It is not a secret if the other neighbouring Kingdoms know about it.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,6 +364,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Docs-Cambria"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -504,64 +509,64 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -879,40 +884,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8367F1B7-398D-4782-AD70-2B5BABC98E37}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="19"/>
+      <c r="F1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="5" t="s">
+      <c r="G1" s="19"/>
+      <c r="H1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="5" t="s">
+      <c r="I1" s="19"/>
+      <c r="J1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="5" t="s">
+      <c r="K1" s="19"/>
+      <c r="L1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="6"/>
+      <c r="M1" s="19"/>
     </row>
-    <row r="2" spans="1:13" ht="42.75">
+    <row r="2" spans="1:13" ht="41.4">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -952,350 +957,345 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1">
-      <c r="A3" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="23" t="s">
+      <c r="A3" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="6"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="19"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="26" t="b">
+      <c r="A4" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="19"/>
+    </row>
+    <row r="5" spans="1:13" ht="152.4">
+      <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" ht="171.75">
-      <c r="A5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="10" t="s">
+    <row r="6" spans="1:13" ht="28.2">
+      <c r="A6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="B6" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="19"/>
+    </row>
+    <row r="7" spans="1:13" ht="28.2">
+      <c r="A7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="B7" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="19"/>
+    </row>
+    <row r="8" spans="1:13" ht="152.4">
+      <c r="A8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="C8" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" ht="29.25">
-      <c r="A6" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="6"/>
+    <row r="9" spans="1:13" ht="28.2">
+      <c r="A9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="19"/>
     </row>
-    <row r="7" spans="1:13" ht="29.25">
-      <c r="A7" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="6"/>
+    <row r="10" spans="1:13" ht="166.2">
+      <c r="A10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" ht="157.5">
-      <c r="A8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="L8" s="11" t="s">
+    <row r="11" spans="1:13" ht="28.2">
+      <c r="A11" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="B11" s="23" t="s">
         <v>48</v>
       </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="19"/>
     </row>
-    <row r="9" spans="1:13" ht="29.25">
-      <c r="A9" s="13" t="s">
+    <row r="12" spans="1:13" ht="138.6">
+      <c r="A12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="C12" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="6"/>
+      <c r="D12" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" ht="171.75">
-      <c r="A10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" s="10" t="s">
+    <row r="13" spans="1:13" ht="28.2">
+      <c r="A13" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="B13" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="19"/>
+    </row>
+    <row r="14" spans="1:13" ht="166.2">
+      <c r="A14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="D14" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="M10" s="10" t="s">
+      <c r="E14" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="29.25">
-      <c r="A11" s="13" t="s">
+      <c r="H14" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="I14" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="6"/>
-    </row>
-    <row r="12" spans="1:13" ht="143.25">
-      <c r="A12" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="16" t="s">
+      <c r="J14" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="K14" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="L14" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="K12" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="L12" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="M12" s="18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="29.25">
-      <c r="A13" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="6"/>
-    </row>
-    <row r="14" spans="1:13" ht="171.75">
-      <c r="A14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="L14" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="M14" s="10" t="s">
-        <v>90</v>
+      <c r="M14" s="26" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="B7:M7"/>
-    <mergeCell ref="B9:M9"/>
     <mergeCell ref="B11:M11"/>
     <mergeCell ref="B13:M13"/>
     <mergeCell ref="L1:M1"/>
@@ -1304,7 +1304,13 @@
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="B7:M7"/>
+    <mergeCell ref="B9:M9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added event summary for WMD
</commit_message>
<xml_diff>
--- a/Stories/WMDs.xlsx
+++ b/Stories/WMDs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ianch\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School Related\DECO3801\DECO3801-Synergistiscs\Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610F1281-E5B0-457B-B692-F4D64A078FED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F197E9-98D4-410B-AF5A-5E3DD8F48A81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{19A45076-EEA2-4D9B-A3FE-00F263EB5362}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{19A45076-EEA2-4D9B-A3FE-00F263EB5362}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="102">
   <si>
     <t>MILITARY</t>
   </si>
@@ -310,6 +310,36 @@
   </si>
   <si>
     <t>It is not a secret if the other neighbouring Kingdoms know about it.</t>
+  </si>
+  <si>
+    <t>EVENT SUMMARY HEADER</t>
+  </si>
+  <si>
+    <t>ACTION 1 EVENT SUMMARY</t>
+  </si>
+  <si>
+    <t>ACTION 2 EVENT SUMMARY</t>
+  </si>
+  <si>
+    <t>ACTION 3 EVENT SUMMARY</t>
+  </si>
+  <si>
+    <t>ACTION 4 EVENT SUMMARY</t>
+  </si>
+  <si>
+    <t>Turns out the neighbouring Kingdom was developing new technology to improve the quality of their equipment and was intending to share this information with other Kingdoms once it is completed.</t>
+  </si>
+  <si>
+    <t>The neighbouring Kingdom was outraged when they caught your spy, implying the amount of distrust you had. This had worsened the mutal ties between the Kingdom.</t>
+  </si>
+  <si>
+    <t>During the meeting, the military commander of the neighbouring Kingdom assured you that are not producing weapons with the aim of attacking other Kingdoms. Although you could sense a little displeasure in their tone due to your insistent probing.</t>
+  </si>
+  <si>
+    <t>The news of your soldiers raiding the neighbouring Kingdom's weapons facility reached the ears of the King from the neighbouring Kingdom. He had seen this move as a call for war and decides to wage war against you.</t>
+  </si>
+  <si>
+    <t>Word of your weapons facility had spread far and wide throughout the neighbouring Kingdoms and they had all seen this as a threat. As such, they have all decided to make an alliance to wage war on you in fear of you getting too powerful.</t>
   </si>
 </sst>
 </file>
@@ -495,7 +525,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -541,11 +571,23 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -555,17 +597,8 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -882,40 +915,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8367F1B7-398D-4782-AD70-2B5BABC98E37}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1"/>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="24" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="24" t="s">
+      <c r="E1" s="20"/>
+      <c r="F1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="24" t="s">
+      <c r="G1" s="20"/>
+      <c r="H1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="24" t="s">
+      <c r="I1" s="20"/>
+      <c r="J1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="19"/>
-      <c r="L1" s="24" t="s">
+      <c r="K1" s="20"/>
+      <c r="L1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="19"/>
+      <c r="M1" s="20"/>
     </row>
     <row r="2" spans="1:13" ht="41.4">
       <c r="A2" s="2"/>
@@ -960,39 +993,39 @@
       <c r="A3" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="20"/>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="20"/>
     </row>
     <row r="5" spans="1:13" ht="152.4">
       <c r="A5" s="5" t="s">
@@ -1039,39 +1072,39 @@
       <c r="A6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="20"/>
     </row>
     <row r="7" spans="1:13" ht="28.2">
       <c r="A7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="20"/>
     </row>
     <row r="8" spans="1:13" ht="152.4">
       <c r="A8" s="5" t="s">
@@ -1118,20 +1151,20 @@
       <c r="A9" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="20"/>
     </row>
     <row r="10" spans="1:13" ht="166.2">
       <c r="A10" s="5" t="s">
@@ -1178,20 +1211,20 @@
       <c r="A11" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="20"/>
     </row>
     <row r="12" spans="1:13" ht="138.6">
       <c r="A12" s="11" t="s">
@@ -1238,20 +1271,20 @@
       <c r="A13" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="20"/>
     </row>
     <row r="14" spans="1:13" ht="166.2">
       <c r="A14" s="5" t="s">
@@ -1266,10 +1299,10 @@
       <c r="D14" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="17" t="s">
         <v>90</v>
       </c>
       <c r="G14" s="6" t="s">
@@ -1290,12 +1323,112 @@
       <c r="L14" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="M14" s="26" t="s">
+      <c r="M14" s="17" t="s">
         <v>91</v>
       </c>
     </row>
+    <row r="15" spans="1:13" ht="55.2">
+      <c r="A15" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="20"/>
+    </row>
+    <row r="16" spans="1:13" ht="55.2">
+      <c r="A16" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="20"/>
+    </row>
+    <row r="17" spans="1:13" ht="55.2">
+      <c r="A17" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="20"/>
+    </row>
+    <row r="18" spans="1:13" ht="55.2">
+      <c r="A18" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="20"/>
+    </row>
+    <row r="19" spans="1:13" ht="55.2">
+      <c r="A19" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="20"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="18">
+    <mergeCell ref="B15:M15"/>
+    <mergeCell ref="B16:M16"/>
+    <mergeCell ref="B17:M17"/>
+    <mergeCell ref="B18:M18"/>
+    <mergeCell ref="B19:M19"/>
     <mergeCell ref="B11:M11"/>
     <mergeCell ref="B13:M13"/>
     <mergeCell ref="L1:M1"/>

</xml_diff>